<commit_message>
bahan jadi is done
</commit_message>
<xml_diff>
--- a/public/template-raw-materals.xlsx
+++ b/public/template-raw-materals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E84627-176D-0F43-9E7C-2839B52CCD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFF520C-D0F8-7A4C-B676-2751B94120A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{7518A780-8C7C-49F0-AF96-CB417392CB7C}"/>
+    <workbookView xWindow="2940" yWindow="500" windowWidth="22660" windowHeight="14260" xr2:uid="{7518A780-8C7C-49F0-AF96-CB417392CB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Item</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Type Of Inventory</t>
+  </si>
+  <si>
+    <t>Raw Material</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
 </sst>
 </file>
@@ -422,7 +428,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -459,7 +465,27 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -475,6 +501,7 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>